<commit_message>
FR - Enter Flight Details created
</commit_message>
<xml_diff>
--- a/Booking System/Create New Order/Default.xlsx
+++ b/Booking System/Create New Order/Default.xlsx
@@ -12,7 +12,7 @@
     <sheet name="FR - Select Flight" sheetId="3" r:id="rId3"/>
     <sheet name="FR - Enter Passenger Details" sheetId="4" r:id="rId4"/>
     <sheet name="FR - Close App" sheetId="5" r:id="rId5"/>
-    <sheet name="FR - Enter Flight Details" sheetId="6" r:id="rId6"/>
+    <sheet name="FR - Find a Flight" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -509,7 +509,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.1"/>

</xml_diff>